<commit_message>
Made final V1.4 revisions
</commit_message>
<xml_diff>
--- a/Documentation/prox_system/prox_module_BOM.xlsx
+++ b/Documentation/prox_system/prox_module_BOM.xlsx
@@ -729,6 +729,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:P182"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -738,16 +741,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="82.28515625" customWidth="1"/>
-    <col min="9" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="81.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" customWidth="1"/>
     <col min="12" max="15" width="12" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
@@ -1565,7 +1569,7 @@
     <hyperlink ref="H15" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId46"/>
+  <pageSetup scale="51" orientation="landscape" r:id="rId46"/>
   <tableParts count="1">
     <tablePart r:id="rId47"/>
   </tableParts>

</xml_diff>